<commit_message>
Changed switch configuration, generated gerbers
Switch now connects directly to bottom side of PCB instead of being
wired to pads. Horizontal SPDT switch selected.

New gerbers generated with Seeed Studio CAM file.
</commit_message>
<xml_diff>
--- a/Hardware/Datasheets and Reference/BOM.xlsx
+++ b/Hardware/Datasheets and Reference/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pin with a Screen Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EAGLE-7.6.0\projects\Pin with a Screen\Hardware\Datasheets and Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
   <si>
     <t>Qty</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Column1</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
     <t>CAP0603-CAP</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>5R</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -236,9 +230,6 @@
     <t>Momentary Switch</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>LED0603</t>
   </si>
   <si>
@@ -318,13 +309,31 @@
   </si>
   <si>
     <t>soldering paste/flux</t>
+  </si>
+  <si>
+    <t>51R</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>solder paste bottle</t>
+  </si>
+  <si>
+    <t>solder</t>
+  </si>
+  <si>
+    <t>loupe tool</t>
+  </si>
+  <si>
+    <t>0.1uF (100nF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +341,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +362,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,15 +377,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,28 +755,28 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -760,28 +785,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -790,28 +815,28 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -820,88 +845,88 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
+      <c r="G7" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -910,28 +935,28 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -940,28 +965,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -970,28 +995,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1000,58 +1025,58 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="G12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1060,28 +1085,28 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1090,28 +1115,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1120,28 +1145,28 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1150,28 +1175,28 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1180,28 +1205,28 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1210,28 +1235,28 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1240,28 +1265,28 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1270,28 +1295,28 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1300,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1309,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1320,18 +1345,38 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="C26" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="C28" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed horizontal button position
Moved horizontal button inwards so that it doesn't stick out so much.
</commit_message>
<xml_diff>
--- a/Hardware/Datasheets and Reference/BOM.xlsx
+++ b/Hardware/Datasheets and Reference/BOM.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
   <si>
     <t>Qty</t>
   </si>
@@ -311,9 +311,6 @@
     <t>soldering paste/flux</t>
   </si>
   <si>
-    <t>51R</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -327,6 +324,12 @@
   </si>
   <si>
     <t>0.1uF (100nF)</t>
+  </si>
+  <si>
+    <t>electronics tweezers</t>
+  </si>
+  <si>
+    <t>56R</t>
   </si>
 </sst>
 </file>
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -935,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
@@ -1205,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>64</v>
@@ -1364,19 +1367,31 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="C26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
+      <c r="B28">
+        <v>1</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>